<commit_message>
Fix d'image DPF + demo d'ajout de fichier
</commit_message>
<xml_diff>
--- a/Remises/DPF.xlsx
+++ b/Remises/DPF.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles-Olivier\Documents\design3\Remises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles-Olivier\Documents\Ulaval\Hiver 2016\Remises\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,12 +56,6 @@
     <t>Signaler une alerte en cas de danger</t>
   </si>
   <si>
-    <t>Afficher les trajectoires (prévue et réelle) sur une vue schématique de la table</t>
-  </si>
-  <si>
-    <t>Communiquer entre l'ordinateur du robot et le microcontrôlleur par UART</t>
-  </si>
-  <si>
     <t>Communiquer sans fil entre l'ordinateur du robot et la station de base</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>Tension entre 21V et 30V</t>
+  </si>
+  <si>
+    <t>Afficher les trajectoires (prévue et réelle) sur une image de la table</t>
+  </si>
+  <si>
+    <t>Communiquer entre l'ordinateur du robot et le microcontrôlleur</t>
   </si>
 </sst>
 </file>
@@ -597,6 +597,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,9 +617,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -898,33 +898,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="C1:AG18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C1:AG18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:AG18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="78.28515625" customWidth="1"/>
+    <col min="3" max="3" width="78.26953125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" customWidth="1"/>
+    <col min="18" max="18" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="D1" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
+    <row r="1" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="D1" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
       <c r="L1" s="15"/>
       <c r="M1" s="16" t="s">
         <v>7</v>
@@ -932,85 +935,85 @@
       <c r="N1" s="17"/>
       <c r="O1" s="15"/>
       <c r="P1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="31" t="s">
+      <c r="S1" s="34"/>
+      <c r="T1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="31" t="s">
+      <c r="U1" s="33"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="34"/>
     </row>
-    <row r="2" spans="3:33" x14ac:dyDescent="0.25">
-      <c r="D2" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+    <row r="2" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="D2" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="36"/>
+      <c r="K2" s="37"/>
       <c r="L2" s="18"/>
       <c r="M2" s="2"/>
       <c r="N2" s="19"/>
       <c r="O2" s="18"/>
       <c r="P2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="24"/>
-      <c r="R2" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="36"/>
+      <c r="R2" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="37"/>
       <c r="T2" s="18"/>
       <c r="U2" s="2"/>
       <c r="V2" s="19"/>
-      <c r="W2" s="34" t="s">
+      <c r="W2" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
     </row>
-    <row r="3" spans="3:33" ht="380.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:33" ht="331" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D3" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>8</v>
@@ -1019,55 +1022,55 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="Q3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="U3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="W3" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>2</v>
@@ -1076,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="Z3" s="8" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="AA3" s="5" t="s">
         <v>6</v>
@@ -1088,21 +1091,21 @@
         <v>5</v>
       </c>
       <c r="AD3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG3" s="9" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C4" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="27"/>
@@ -1159,9 +1162,9 @@
       <c r="AF4" s="27"/>
       <c r="AG4" s="28"/>
     </row>
-    <row r="5" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C5" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="10">
         <v>5</v>
@@ -1210,7 +1213,7 @@
       <c r="AF5" s="7"/>
       <c r="AG5" s="11"/>
     </row>
-    <row r="6" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C6" s="29" t="s">
         <v>1</v>
       </c>
@@ -1251,9 +1254,9 @@
       <c r="AF6" s="7"/>
       <c r="AG6" s="11"/>
     </row>
-    <row r="7" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C7" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="7"/>
@@ -1290,9 +1293,9 @@
       <c r="AF7" s="7"/>
       <c r="AG7" s="11"/>
     </row>
-    <row r="8" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C8" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="7"/>
@@ -1331,9 +1334,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C9" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="7"/>
@@ -1368,9 +1371,9 @@
       <c r="AF9" s="7"/>
       <c r="AG9" s="11"/>
     </row>
-    <row r="10" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C10" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="7"/>
@@ -1407,9 +1410,9 @@
       <c r="AF10" s="7"/>
       <c r="AG10" s="11"/>
     </row>
-    <row r="11" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C11" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="10">
         <v>4</v>
@@ -1448,9 +1451,9 @@
       <c r="AF11" s="7"/>
       <c r="AG11" s="11"/>
     </row>
-    <row r="12" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C12" s="29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="7">
@@ -1495,9 +1498,9 @@
       <c r="AF12" s="7"/>
       <c r="AG12" s="11"/>
     </row>
-    <row r="13" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C13" s="29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="7"/>
@@ -1544,9 +1547,9 @@
       <c r="AF13" s="7"/>
       <c r="AG13" s="11"/>
     </row>
-    <row r="14" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C14" s="29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="7"/>
@@ -1583,9 +1586,9 @@
       <c r="AF14" s="7"/>
       <c r="AG14" s="11"/>
     </row>
-    <row r="15" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C15" s="29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="10">
         <v>1</v>
@@ -1660,9 +1663,9 @@
       <c r="AF15" s="7"/>
       <c r="AG15" s="11"/>
     </row>
-    <row r="16" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:33" x14ac:dyDescent="0.35">
       <c r="C16" s="29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="7"/>
@@ -1699,9 +1702,9 @@
       <c r="AF16" s="7"/>
       <c r="AG16" s="11"/>
     </row>
-    <row r="17" spans="3:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="12">
         <v>4</v>
@@ -1742,22 +1745,16 @@
       <c r="AF17" s="13"/>
       <c r="AG17" s="14"/>
     </row>
-    <row r="18" spans="3:33" ht="123" x14ac:dyDescent="0.25">
-      <c r="D18" s="37" t="s">
-        <v>60</v>
+    <row r="18" spans="3:33" ht="119.5" x14ac:dyDescent="0.35">
+      <c r="D18" s="31" t="s">
+        <v>58</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="R1:S1"/>
@@ -1765,8 +1762,15 @@
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="Z2:AC2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="37" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
transition DPF vers tour pour continuer travail
</commit_message>
<xml_diff>
--- a/Remises/DPF.xlsx
+++ b/Remises/DPF.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Manipuler les trésors</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Actualiser affichage à une fréquence minimale de 0.2Hz</t>
   </si>
   <si>
-    <t>Affichage de la tension du condensateur en temps réel sur la station de base</t>
-  </si>
-  <si>
     <t>Finir le projet d'ici le 17 avril.</t>
   </si>
   <si>
@@ -207,6 +204,18 @@
   </si>
   <si>
     <t>Communiquer entre l'ordinateur du robot et le microcontrôlleur</t>
+  </si>
+  <si>
+    <t>Affichage de la tension du condensateur et de la trajectoire planifiée, de la position et de l'orientation du robot  en temps réel sur la station de base</t>
+  </si>
+  <si>
+    <t>Activer la routine au démarrage du micro-PC sans requête extérieure</t>
+  </si>
+  <si>
+    <t>Communiquer sans-fil un message secret avec un encodage Manchester</t>
+  </si>
+  <si>
+    <t>Obtenir une île cible du serveur des îles</t>
   </si>
 </sst>
 </file>
@@ -539,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -618,6 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,15 +911,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:AG18"/>
+  <dimension ref="C1:AG29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:AG18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="78.26953125" customWidth="1"/>
+    <col min="3" max="3" width="120.90625" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="10" max="10" width="9.1796875" customWidth="1"/>
     <col min="18" max="18" width="10.453125" customWidth="1"/>
@@ -917,14 +927,14 @@
   <sheetData>
     <row r="1" spans="3:33" x14ac:dyDescent="0.35">
       <c r="D1" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
       <c r="H1" s="34"/>
       <c r="I1" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" s="33"/>
       <c r="K1" s="34"/>
@@ -935,11 +945,11 @@
       <c r="N1" s="17"/>
       <c r="O1" s="15"/>
       <c r="P1" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="23"/>
       <c r="R1" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S1" s="34"/>
       <c r="T1" s="32" t="s">
@@ -948,18 +958,18 @@
       <c r="U1" s="33"/>
       <c r="V1" s="34"/>
       <c r="W1" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X1" s="33"/>
       <c r="Y1" s="34"/>
       <c r="Z1" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="33"/>
       <c r="AB1" s="33"/>
       <c r="AC1" s="34"/>
       <c r="AD1" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE1" s="33"/>
       <c r="AF1" s="33"/>
@@ -967,14 +977,14 @@
     </row>
     <row r="2" spans="3:33" x14ac:dyDescent="0.35">
       <c r="D2" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
       <c r="H2" s="37"/>
       <c r="I2" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" s="36"/>
       <c r="K2" s="37"/>
@@ -983,29 +993,29 @@
       <c r="N2" s="19"/>
       <c r="O2" s="18"/>
       <c r="P2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="24"/>
       <c r="R2" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S2" s="37"/>
       <c r="T2" s="18"/>
       <c r="U2" s="2"/>
       <c r="V2" s="19"/>
       <c r="W2" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X2" s="36"/>
       <c r="Y2" s="37"/>
       <c r="Z2" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA2" s="36"/>
       <c r="AB2" s="36"/>
       <c r="AC2" s="37"/>
       <c r="AD2" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AE2" s="36"/>
       <c r="AF2" s="36"/>
@@ -1013,7 +1023,7 @@
     </row>
     <row r="3" spans="3:33" ht="331" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>8</v>
@@ -1022,10 +1032,10 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>20</v>
@@ -1034,43 +1044,43 @@
         <v>21</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="20" t="s">
         <v>13</v>
       </c>
       <c r="M3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="21" t="s">
-        <v>32</v>
-      </c>
       <c r="O3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="Q3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="T3" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="U3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="V3" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>2</v>
@@ -1079,7 +1089,7 @@
         <v>3</v>
       </c>
       <c r="Z3" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA3" s="5" t="s">
         <v>6</v>
@@ -1091,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="AD3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE3" s="5" t="s">
         <v>10</v>
@@ -1294,467 +1304,488 @@
       <c r="AG7" s="11"/>
     </row>
     <row r="8" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C9" s="38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C10" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="7">
-        <v>5</v>
-      </c>
-      <c r="AF8" s="7">
-        <v>5</v>
-      </c>
-      <c r="AG8" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C9" s="29" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="7">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="7">
+        <v>5</v>
+      </c>
+      <c r="AG18" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C19" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="11">
+        <v>5</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="11"/>
+    </row>
+    <row r="20" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C20" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7">
+        <v>5</v>
+      </c>
+      <c r="H20" s="11">
+        <v>5</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="11"/>
+    </row>
+    <row r="21" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C21" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="10">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="11">
+        <v>2</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="7">
+        <v>3</v>
+      </c>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="11"/>
+    </row>
+    <row r="22" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="7">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="7">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="10">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="7"/>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="11"/>
+    </row>
+    <row r="23" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C23" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="10">
+        <v>2</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="10">
+        <v>4</v>
+      </c>
+      <c r="P23" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>4</v>
+      </c>
+      <c r="R23" s="10"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="10">
+        <v>3</v>
+      </c>
+      <c r="U23" s="7">
+        <v>3</v>
+      </c>
+      <c r="V23" s="11">
+        <v>3</v>
+      </c>
+      <c r="W23" s="10"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="11"/>
+    </row>
+    <row r="24" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C24" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="10"/>
+      <c r="AE24" s="7">
+        <v>5</v>
+      </c>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="11"/>
+    </row>
+    <row r="25" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C25" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7">
+        <v>2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>2</v>
+      </c>
+      <c r="G25" s="7">
+        <v>2</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1</v>
+      </c>
+      <c r="I25" s="10">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7">
+        <v>2</v>
+      </c>
+      <c r="K25" s="11">
+        <v>2</v>
+      </c>
+      <c r="L25" s="10">
+        <v>2</v>
+      </c>
+      <c r="M25" s="7">
+        <v>2</v>
+      </c>
+      <c r="N25" s="11">
+        <v>2</v>
+      </c>
+      <c r="O25" s="10">
+        <v>5</v>
+      </c>
+      <c r="P25" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>5</v>
+      </c>
+      <c r="R25" s="10">
+        <v>4</v>
+      </c>
+      <c r="S25" s="11">
+        <v>4</v>
+      </c>
+      <c r="T25" s="10">
+        <v>4</v>
+      </c>
+      <c r="U25" s="7">
+        <v>4</v>
+      </c>
+      <c r="V25" s="11">
+        <v>4</v>
+      </c>
+      <c r="W25" s="10">
+        <v>3</v>
+      </c>
+      <c r="X25" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="10"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="11"/>
+    </row>
+    <row r="26" spans="3:33" x14ac:dyDescent="0.35">
+      <c r="C26" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="10">
+        <v>5</v>
+      </c>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="10"/>
+      <c r="AA26" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="10"/>
+      <c r="AE26" s="7"/>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="11"/>
+    </row>
+    <row r="27" spans="3:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C27" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="11">
-        <v>5</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="7"/>
-      <c r="AF9" s="7"/>
-      <c r="AG9" s="11"/>
-    </row>
-    <row r="10" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C10" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7">
-        <v>5</v>
-      </c>
-      <c r="H10" s="11">
-        <v>5</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="7"/>
-      <c r="AF10" s="7"/>
-      <c r="AG10" s="11"/>
-    </row>
-    <row r="11" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C11" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="D27" s="12">
         <v>4</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="11">
-        <v>2</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="10"/>
-      <c r="AE11" s="7">
+      <c r="E27" s="13"/>
+      <c r="F27" s="13">
+        <v>4</v>
+      </c>
+      <c r="G27" s="13">
         <v>3</v>
       </c>
-      <c r="AF11" s="7"/>
-      <c r="AG11" s="11"/>
-    </row>
-    <row r="12" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="7">
-        <v>5</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="7">
-        <v>5</v>
-      </c>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="10">
-        <v>5</v>
-      </c>
-      <c r="AA12" s="7">
-        <v>5</v>
-      </c>
-      <c r="AB12" s="7">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="11">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="10"/>
-      <c r="AE12" s="7"/>
-      <c r="AF12" s="7"/>
-      <c r="AG12" s="11"/>
-    </row>
-    <row r="13" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10">
-        <v>2</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="10">
+      <c r="H27" s="14">
         <v>4</v>
       </c>
-      <c r="P13" s="7">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="11">
-        <v>4</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="10">
-        <v>3</v>
-      </c>
-      <c r="U13" s="7">
-        <v>3</v>
-      </c>
-      <c r="V13" s="11">
-        <v>3</v>
-      </c>
-      <c r="W13" s="10"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="10"/>
-      <c r="AE13" s="7"/>
-      <c r="AF13" s="7"/>
-      <c r="AG13" s="11"/>
-    </row>
-    <row r="14" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C14" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7">
-        <v>5</v>
-      </c>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="7">
-        <v>5</v>
-      </c>
-      <c r="AF14" s="7"/>
-      <c r="AG14" s="11"/>
-    </row>
-    <row r="15" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C15" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="10">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7">
-        <v>2</v>
-      </c>
-      <c r="F15" s="7">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7">
-        <v>2</v>
-      </c>
-      <c r="H15" s="11">
-        <v>1</v>
-      </c>
-      <c r="I15" s="10">
-        <v>1</v>
-      </c>
-      <c r="J15" s="7">
-        <v>2</v>
-      </c>
-      <c r="K15" s="11">
-        <v>2</v>
-      </c>
-      <c r="L15" s="10">
-        <v>2</v>
-      </c>
-      <c r="M15" s="7">
-        <v>2</v>
-      </c>
-      <c r="N15" s="11">
-        <v>2</v>
-      </c>
-      <c r="O15" s="10">
-        <v>5</v>
-      </c>
-      <c r="P15" s="7">
-        <v>5</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>5</v>
-      </c>
-      <c r="R15" s="10">
-        <v>4</v>
-      </c>
-      <c r="S15" s="11">
-        <v>4</v>
-      </c>
-      <c r="T15" s="10">
-        <v>4</v>
-      </c>
-      <c r="U15" s="7">
-        <v>4</v>
-      </c>
-      <c r="V15" s="11">
-        <v>4</v>
-      </c>
-      <c r="W15" s="10">
-        <v>3</v>
-      </c>
-      <c r="X15" s="7">
-        <v>3</v>
-      </c>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="11"/>
-    </row>
-    <row r="16" spans="3:33" x14ac:dyDescent="0.35">
-      <c r="C16" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="10">
-        <v>5</v>
-      </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="7">
-        <v>5</v>
-      </c>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="7"/>
-      <c r="AF16" s="7"/>
-      <c r="AG16" s="11"/>
-    </row>
-    <row r="17" spans="3:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="12">
-        <v>4</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13">
-        <v>4</v>
-      </c>
-      <c r="G17" s="13">
-        <v>3</v>
-      </c>
-      <c r="H17" s="14">
-        <v>4</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="14"/>
-    </row>
-    <row r="18" spans="3:33" ht="119.5" x14ac:dyDescent="0.35">
-      <c r="D18" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>33</v>
+      <c r="I27" s="12"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="14"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="13"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="14"/>
+    </row>
+    <row r="29" spans="3:33" ht="119.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="R1:S1"/>
@@ -1762,12 +1793,6 @@
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="Z2:AC2"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>